<commit_message>
Author  : vikas files added : VikasMalhotra.xlsx Description  : modified the task division
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikas malohtra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikas malohtra\Desktop\New folder (2)\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>Story ID</t>
   </si>
@@ -54,12 +54,6 @@
     <t>SSDMS-6</t>
   </si>
   <si>
-    <t>Firstly understand the why of the story.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Then I start modifying the code to make the page looks as agred in the GD </t>
-  </si>
-  <si>
     <t xml:space="preserve">Then I make technical understanding where html and css is used </t>
   </si>
   <si>
@@ -70,9 +64,6 @@
   </si>
   <si>
     <t>Firstly I will work on the front end of the sign up page</t>
-  </si>
-  <si>
-    <t>Then I will work on the backend part to send the information to the profile creation page.</t>
   </si>
   <si>
     <t>Then I send my code to QA for tetsing.</t>
@@ -112,6 +103,21 @@
   </si>
   <si>
     <t>T-8</t>
+  </si>
+  <si>
+    <t>Start the development.</t>
+  </si>
+  <si>
+    <t>Then I will work on to post the data on the database</t>
+  </si>
+  <si>
+    <t>T-5.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After getting the response from the database appropriate action will be performed. </t>
+  </si>
+  <si>
+    <t>Firstly understand the  "why" of the story.</t>
   </si>
 </sst>
 </file>
@@ -258,24 +264,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,8 +274,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2868,10 +2874,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,199 +2914,205 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6">
-        <v>40</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="16">
+      <c r="B3" s="14">
+        <v>52</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="15">
+      <c r="G3" s="9">
         <f>E3-F3</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="9">
+        <f t="shared" ref="G4:G47" si="0">E4-F4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="10">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E8" s="10">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="15">
-        <f t="shared" ref="G4:G46" si="0">E4-F4</f>
+      <c r="F11" s="2"/>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="17">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="15">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="17">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="17">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="17">
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="10">
         <v>6</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="15">
+      <c r="F13" s="2"/>
+      <c r="G13" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="17">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="15">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="17">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="17">
-        <v>6</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="15">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3499,10 +3511,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : Vikas malohtra FILES ADDED : VikasMalhotra.xlsx Description : sprint planning sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Story ID</t>
   </si>
@@ -54,25 +54,7 @@
     <t>SSDMS-6</t>
   </si>
   <si>
-    <t xml:space="preserve">Then I make technical understanding where html and css is used </t>
-  </si>
-  <si>
-    <t>Then I understand forward and backward linkages .</t>
-  </si>
-  <si>
     <t>Make the block diagram of the entire code journey</t>
-  </si>
-  <si>
-    <t>Firstly I will work on the front end of the sign up page</t>
-  </si>
-  <si>
-    <t>Then I send my code to QA for tetsing.</t>
-  </si>
-  <si>
-    <t>Then my code is review by the appropriate member.</t>
-  </si>
-  <si>
-    <t>Then I incorporate the code review changes.</t>
   </si>
   <si>
     <t>T-1</t>
@@ -99,25 +81,31 @@
     <t>T-6</t>
   </si>
   <si>
-    <t>T-7</t>
-  </si>
-  <si>
-    <t>T-8</t>
-  </si>
-  <si>
     <t>Start the development.</t>
-  </si>
-  <si>
-    <t>Then I will work on to post the data on the database</t>
   </si>
   <si>
     <t>T-5.3</t>
   </si>
   <si>
-    <t xml:space="preserve">After getting the response from the database appropriate action will be performed. </t>
+    <t>Understand the  "why" of the story.</t>
   </si>
   <si>
-    <t>Firstly understand the  "why" of the story.</t>
+    <t>Understand forward and backward linkages .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make technical understanding where html and css is used </t>
+  </si>
+  <si>
+    <t>Work on to post the data on the backend</t>
+  </si>
+  <si>
+    <t>Review and incorporate the changes</t>
+  </si>
+  <si>
+    <t>work on the front end of the sign up page</t>
+  </si>
+  <si>
+    <t>Receive data from the back end and send to the appropriate role.</t>
   </si>
 </sst>
 </file>
@@ -185,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -232,24 +220,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -275,13 +250,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -290,10 +263,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2874,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G47"/>
+  <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,19 +2883,19 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="14">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="17">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
@@ -2936,31 +2905,31 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="15"/>
       <c r="C4" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="9">
-        <f t="shared" ref="G4:G47" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G45" si="0">E4-F4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
@@ -2972,13 +2941,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="15"/>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E6" s="10">
         <v>4</v>
@@ -2990,13 +2959,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="15"/>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E7" s="10">
         <v>36</v>
@@ -3008,13 +2977,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="15"/>
       <c r="C8" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E8" s="10">
         <v>6</v>
@@ -3026,13 +2995,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E9" s="10">
         <v>18</v>
@@ -3043,14 +3012,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
       <c r="B10" s="15"/>
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="10">
         <v>12</v>
@@ -3062,13 +3031,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="15"/>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -3080,39 +3049,27 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="10">
-        <v>6</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3499,34 +3456,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author   : Vikas Files added  : VikasMalhotra.xlsx Description  : updated file of sprint sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Story ID</t>
   </si>
@@ -72,19 +72,7 @@
     <t>T-5</t>
   </si>
   <si>
-    <t>T-5.1</t>
-  </si>
-  <si>
-    <t>T-5.2</t>
-  </si>
-  <si>
     <t>T-6</t>
-  </si>
-  <si>
-    <t>Start the development.</t>
-  </si>
-  <si>
-    <t>T-5.3</t>
   </si>
   <si>
     <t>Understand the  "why" of the story.</t>
@@ -96,16 +84,37 @@
     <t xml:space="preserve">Make technical understanding where html and css is used </t>
   </si>
   <si>
-    <t>Work on to post the data on the backend</t>
-  </si>
-  <si>
     <t>Review and incorporate the changes</t>
   </si>
   <si>
-    <t>work on the front end of the sign up page</t>
+    <t>Type</t>
   </si>
   <si>
-    <t>Receive data from the back end and send to the appropriate role.</t>
+    <t>Development of signup page</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Understand forward and backward linkages</t>
+  </si>
+  <si>
+    <t>Understand the angular services</t>
+  </si>
+  <si>
+    <t>Write code to post the data on backend</t>
+  </si>
+  <si>
+    <t>Understand the response from the backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write the code to route the user to the page according to their role </t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -129,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +181,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -220,11 +253,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +342,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2843,623 +2953,595 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G45"/>
+  <dimension ref="A2:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="67.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14">
-        <v>45</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="14">
+        <f>SUM(F3:F8)</f>
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="9">
-        <f>E3-F3</f>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <f>F3-G3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="6" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="9">
+        <f t="shared" ref="H4:H8" si="0">F4-G4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F7" s="10">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="9">
-        <f t="shared" ref="G4:G45" si="0">E4-F4</f>
+      <c r="G8" s="2"/>
+      <c r="H8" s="9">
+        <f>F8-G8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14">
+        <v>8</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <f>F10-G10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="9">
+        <f t="shared" ref="H11:H13" si="1">F11-G11</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="6" t="s">
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="14">
+        <v>6</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="9">
+        <f>F15-G15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="10">
         <v>4</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="9">
-        <f t="shared" si="0"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="9">
+        <f t="shared" ref="H16:H17" si="2">F16-G16</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="10">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="10">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="10">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="9">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="10">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="F17" s="10">
         <v>1</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="9">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="26">
+        <f>SUM(C3:C17)</f>
+        <v>29</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <f t="shared" ref="H4:H37" si="3">F18-G18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2">
-        <f t="shared" si="0"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:B11"/>
+  <mergeCells count="11">
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
AUTHOR : VIKAS FILES ADDED : VikasMalhotra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -57,24 +57,6 @@
     <t>Make the block diagram of the entire code journey</t>
   </si>
   <si>
-    <t>T-1</t>
-  </si>
-  <si>
-    <t>T-2</t>
-  </si>
-  <si>
-    <t>T-3</t>
-  </si>
-  <si>
-    <t>T-4</t>
-  </si>
-  <si>
-    <t>T-5</t>
-  </si>
-  <si>
-    <t>T-6</t>
-  </si>
-  <si>
     <t>Understand the  "why" of the story.</t>
   </si>
   <si>
@@ -115,6 +97,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
   </si>
 </sst>
 </file>
@@ -330,6 +330,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -342,24 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,10 +370,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2956,7 +2956,7 @@
   <dimension ref="A2:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D15" sqref="D15:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2970,8 +2970,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>19</v>
+      <c r="A2" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2996,21 +2996,21 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="21">
         <f>SUM(F3:F8)</f>
         <v>15</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="11">
         <v>1</v>
@@ -3024,30 +3024,30 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="9">
-        <f t="shared" ref="H4:H8" si="0">F4-G4</f>
+        <f t="shared" ref="H4:H7" si="0">F4-G4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>8</v>
@@ -3062,14 +3062,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
@@ -3081,14 +3081,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F7" s="10">
         <v>6</v>
@@ -3100,14 +3100,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -3119,30 +3119,30 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="21">
         <v>8</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>9</v>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
@@ -3157,13 +3157,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="19" t="s">
-        <v>10</v>
+      <c r="B11" s="20"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
@@ -3176,13 +3176,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="19" t="s">
-        <v>11</v>
+      <c r="B12" s="20"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -3195,13 +3195,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="19" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
@@ -3213,29 +3213,29 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="21">
         <v>6</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>9</v>
+      <c r="D15" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
@@ -3248,13 +3248,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="19" t="s">
-        <v>10</v>
+      <c r="B16" s="20"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F16" s="10">
         <v>4</v>
@@ -3267,13 +3267,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="19" t="s">
-        <v>11</v>
+      <c r="B17" s="20"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
@@ -3285,10 +3285,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="26">
+      <c r="B18" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="15">
         <f>SUM(C3:C17)</f>
         <v>29</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2">
-        <f t="shared" ref="H4:H37" si="3">F18-G18</f>
+        <f t="shared" ref="H18:H37" si="3">F18-G18</f>
         <v>0</v>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B14:H14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
AUTHOR : Vikas malohtra FILES ADDED : VikasMalhotra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Story ID</t>
   </si>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">write the code to route the user to the page according to their role </t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -114,7 +111,10 @@
     <t>T5</t>
   </si>
   <si>
-    <t>T6</t>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -138,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +202,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -336,16 +348,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -361,6 +363,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,8 +381,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2953,10 +2976,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H37"/>
+  <dimension ref="A2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,18 +3019,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21">
-        <f>SUM(F3:F8)</f>
-        <v>15</v>
+      <c r="C3" s="17">
+        <f>SUM(F3:F7)</f>
+        <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>9</v>
@@ -3024,11 +3047,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>10</v>
@@ -3043,11 +3066,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>8</v>
@@ -3062,11 +3085,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
@@ -3081,11 +3104,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>14</v>
@@ -3100,211 +3123,204 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="10">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="9">
-        <f>F8-G8</f>
-        <v>1</v>
-      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17">
+        <v>7</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <f>F9-G9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="21">
-        <v>8</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="9">
-        <f>F10-G10</f>
-        <v>1</v>
+        <f t="shared" ref="H10:H12" si="1">F10-G10</f>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="22"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="9">
-        <f t="shared" ref="H11:H13" si="1">F11-G11</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="22"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F12" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="10">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="17">
+        <v>5</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="10">
         <v>1</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="9">
-        <f t="shared" si="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="9">
+        <f>F14-G14</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-    </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="21">
-        <v>6</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="9">
-        <f>F15-G15</f>
-        <v>1</v>
+        <f t="shared" ref="H15" si="2">F15-G15</f>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="10">
-        <v>4</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="9">
-        <f t="shared" ref="H16:H17" si="2">F16-G16</f>
-        <v>4</v>
-      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="13" t="s">
-        <v>25</v>
+      <c r="A17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="25">
+        <v>2</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="10">
-        <v>1</v>
+      <c r="F17" s="29">
+        <v>2</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" ref="H16:H34" si="3">F17-G17</f>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="15">
-        <f>SUM(C3:C17)</f>
-        <v>29</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2">
-        <f t="shared" ref="H18:H37" si="3">F18-G18</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="31">
+        <v>28</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -3493,55 +3509,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B14:H14"/>
+  <mergeCells count="12">
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
AUTHOR : Vikas FIKES ADDED : VikasMalhotra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikas malohtra\Desktop\New folder (2)\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017.git\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -348,6 +348,30 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -371,30 +395,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2978,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3019,13 +3019,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="27">
         <f>SUM(F3:F7)</f>
         <v>14</v>
       </c>
@@ -3039,17 +3039,17 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="9">
         <f>F3-G3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
@@ -3059,16 +3059,18 @@
       <c r="F4" s="10">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
       <c r="H4" s="9">
         <f t="shared" ref="H4:H7" si="0">F4-G4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="18"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
@@ -3078,16 +3080,18 @@
       <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
@@ -3097,16 +3101,18 @@
       <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>4</v>
+      </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
@@ -3123,23 +3129,23 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="27">
         <v>7</v>
       </c>
       <c r="D9" s="13" t="s">
@@ -3160,9 +3166,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="13" t="s">
         <v>23</v>
       </c>
@@ -3179,9 +3185,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="13" t="s">
         <v>24</v>
       </c>
@@ -3198,9 +3204,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
@@ -3217,22 +3223,22 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="27">
         <v>5</v>
       </c>
       <c r="D14" s="13" t="s">
@@ -3251,9 +3257,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="13" t="s">
         <v>23</v>
       </c>
@@ -3270,34 +3276,34 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="14">
         <v>2</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="18">
         <v>2</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="9">
-        <f t="shared" ref="H16:H34" si="3">F17-G17</f>
+        <f t="shared" ref="H17:H34" si="3">F17-G17</f>
         <v>2</v>
       </c>
     </row>
@@ -3315,10 +3321,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="20">
         <v>28</v>
       </c>
       <c r="E19" s="3"/>

</xml_diff>

<commit_message>
AUTHOR : VIKAS FILES MODIFIED  : VikasMalhotra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
+++ b/TeamDetails/TasksBreakDown/VikasMalhotra.xlsx
@@ -120,12 +120,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>In Dev</t>
-  </si>
-  <si>
-    <t>Not statrted</t>
-  </si>
-  <si>
     <t>Not statred</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>Hours Needed</t>
+  </si>
+  <si>
+    <t>In QA</t>
+  </si>
+  <si>
+    <t>IN DEV</t>
   </si>
 </sst>
 </file>
@@ -3033,7 +3033,7 @@
   <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3203,7 +3203,7 @@
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
       <c r="G8" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H8" s="25">
         <f>SUM(H3:H7)</f>
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3254,11 +3254,11 @@
         <v>3</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" ref="H10:H12" si="1">F10-G10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="32"/>
     </row>
@@ -3275,10 +3275,12 @@
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
       <c r="H11" s="9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11" s="32"/>
     </row>
@@ -3309,11 +3311,11 @@
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H13" s="29">
         <f>SUM(H9:H12)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3341,7 +3343,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3371,7 +3373,7 @@
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H16" s="31">
         <f>SUM(H14:H15)</f>
@@ -3401,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>